<commit_message>
added keys to .gitignore
</commit_message>
<xml_diff>
--- a/Google Calendar Notes v02.xlsb.xlsx
+++ b/Google Calendar Notes v02.xlsb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\My Documents\code\python\Pycharm Projects\Self Study\GoogleCalendar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02968283-8F92-40F6-998F-BD1A422BBFC4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1980056D-C475-4A8B-A9A6-13F8D0485508}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1886" yWindow="514" windowWidth="16988" windowHeight="13200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4149" yWindow="386" windowWidth="16971" windowHeight="13200" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Todos" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="362">
   <si>
     <t>Notes on learning how the google calendar api works</t>
   </si>
@@ -1058,6 +1058,72 @@
   </si>
   <si>
     <t>launchpad walk through 2/16/21</t>
+  </si>
+  <si>
+    <t>goo.gl/8QbNaZ</t>
+  </si>
+  <si>
+    <t>employee01@tony-held.com</t>
+  </si>
+  <si>
+    <t>employee02@tony-held.com</t>
+  </si>
+  <si>
+    <t>employee03@tony-held.com</t>
+  </si>
+  <si>
+    <t>employee04@tony-held.com</t>
+  </si>
+  <si>
+    <t>employee05@tony-held.com</t>
+  </si>
+  <si>
+    <t>patient01@tony-held.com</t>
+  </si>
+  <si>
+    <t>patient02@tony-held.com</t>
+  </si>
+  <si>
+    <t>patient03@tony-held.com</t>
+  </si>
+  <si>
+    <t>patient04@tony-held.com</t>
+  </si>
+  <si>
+    <t>patient05@tony-held.com</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/calendar/v3/reference/events/watch#request-body</t>
+  </si>
+  <si>
+    <t>calendar watch details</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/42022277/google-calendar-event-created-updated-deleted-webhook</t>
+  </si>
+  <si>
+    <t>https://help.smartrecruiters.com/Integrations/Calendar_integrations/Set_Up_Google_Calendar_Integration</t>
+  </si>
+  <si>
+    <t>https://cloud.google.com/run/docs/triggering/webhooks</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/hangouts/chat/quickstart/incoming-bot-python</t>
+  </si>
+  <si>
+    <t>https://zapier.com/engineering/how-to-use-the-google-calendar-api/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">start here to continue analysis of python anywhere </t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/processing-incoming-request-data-in-flask</t>
+  </si>
+  <si>
+    <t>looks like a good incoming request review</t>
+  </si>
+  <si>
+    <t>https://tedboy.github.io/flask/generated/generated/flask.Request.html</t>
   </si>
 </sst>
 </file>
@@ -1573,10 +1639,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9487F4F7-7C80-47D4-A0C8-78A1120B8919}">
-  <dimension ref="A3:M81"/>
+  <dimension ref="A3:M91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1978,44 +2044,84 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B68" t="s">
+      <c r="G68" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B69" t="s">
         <v>87</v>
       </c>
-      <c r="G68" s="1" t="s">
+      <c r="G69" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B70" t="s">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B71" t="s">
         <v>89</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="G71" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A73" t="s">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A74" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B74" s="1" t="s">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B75" s="1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A76" t="s">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A77" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="B77" s="1" t="s">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="B78" s="1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A81" t="s">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A82" t="s">
         <v>339</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A84" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B85" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B87" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B88" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B89" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B90" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B91" s="1" t="s">
+        <v>357</v>
       </c>
     </row>
   </sheetData>
@@ -2041,10 +2147,10 @@
     <hyperlink ref="G65" r:id="rId19" xr:uid="{D61D591B-EDC2-4670-BC14-3866EFA989F1}"/>
     <hyperlink ref="G66" r:id="rId20" xr:uid="{112D3872-6E2F-44B9-9EAA-7E9FA8A67046}"/>
     <hyperlink ref="G67" r:id="rId21" xr:uid="{FFF3CC53-9D16-4A60-83F1-842871F4A57F}"/>
-    <hyperlink ref="G68" r:id="rId22" xr:uid="{BFF84ABA-2C42-434A-91FB-0DA0CCB078DD}"/>
-    <hyperlink ref="G70" r:id="rId23" xr:uid="{16BB30BB-647A-4A7B-BEAB-781F7C72C926}"/>
-    <hyperlink ref="B74" r:id="rId24" xr:uid="{E32C6B96-067C-4034-811D-8489056DFB4E}"/>
-    <hyperlink ref="B77" r:id="rId25" xr:uid="{F7579AAB-A33D-4E12-8BDD-F1BEF455A012}"/>
+    <hyperlink ref="G69" r:id="rId22" xr:uid="{BFF84ABA-2C42-434A-91FB-0DA0CCB078DD}"/>
+    <hyperlink ref="G71" r:id="rId23" xr:uid="{16BB30BB-647A-4A7B-BEAB-781F7C72C926}"/>
+    <hyperlink ref="B75" r:id="rId24" xr:uid="{E32C6B96-067C-4034-811D-8489056DFB4E}"/>
+    <hyperlink ref="B78" r:id="rId25" xr:uid="{F7579AAB-A33D-4E12-8BDD-F1BEF455A012}"/>
     <hyperlink ref="E9" r:id="rId26" xr:uid="{AFF7A057-F082-44EC-B5FC-BCD9E5B24B32}"/>
     <hyperlink ref="G22" r:id="rId27" xr:uid="{4C617653-AFFC-4339-91A4-3236A9E2C26C}"/>
     <hyperlink ref="E26" r:id="rId28" xr:uid="{73B291DC-D479-4E08-80F4-E2122CFAC64A}"/>
@@ -2053,6 +2159,12 @@
     <hyperlink ref="E19" r:id="rId31" xr:uid="{F769F22C-C2FD-4AA9-8CDF-2BAF384237A4}"/>
     <hyperlink ref="G60" r:id="rId32" xr:uid="{18F94EA3-1C84-4F68-9E04-5B0ACB9AD9C6}"/>
     <hyperlink ref="G61" r:id="rId33" xr:uid="{5E404D0C-1D63-4264-8E58-391ED0BE7ACC}"/>
+    <hyperlink ref="B85" r:id="rId34" location="request-body" xr:uid="{974D4DF0-2683-4DDE-9716-FFA034474393}"/>
+    <hyperlink ref="B87" r:id="rId35" xr:uid="{BF3BDBEA-45C7-4A66-A52C-21464CAA9288}"/>
+    <hyperlink ref="B88" r:id="rId36" xr:uid="{F2EEF78A-BAAD-4292-AC41-A36AF9CF3D68}"/>
+    <hyperlink ref="B89" r:id="rId37" xr:uid="{134B86F6-2B1B-49C5-918E-53322CDB8241}"/>
+    <hyperlink ref="B90" r:id="rId38" xr:uid="{3D827265-B019-4B37-B8F8-0437D7FE9E1B}"/>
+    <hyperlink ref="B91" r:id="rId39" xr:uid="{DE22239A-97D4-45A3-A1D9-A9C15074D7E8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2060,10 +2172,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBA689AE-B311-4575-B246-96F524D0AFBF}">
-  <dimension ref="A5:P132"/>
+  <dimension ref="A5:P135"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -2177,6 +2289,9 @@
       <c r="B30" s="1" t="s">
         <v>181</v>
       </c>
+      <c r="I30" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B31" s="1"/>
@@ -2187,7 +2302,7 @@
       </c>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B33" s="1" t="s">
         <v>165</v>
       </c>
@@ -2196,38 +2311,30 @@
       </c>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>222</v>
       </c>
       <c r="B35" s="1"/>
-      <c r="K35" s="1"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B36" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="I36" t="s">
         <v>223</v>
       </c>
-      <c r="J36" s="9"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="9"/>
-      <c r="M36" s="9"/>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="K37" s="1"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B39" s="1" t="s">
         <v>104</v>
       </c>
@@ -2235,46 +2342,46 @@
         <v>217</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B40" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B41" s="1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B42" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B43" s="1" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B44" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>175</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B47" s="1" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B48" s="1" t="s">
         <v>184</v>
       </c>
@@ -2531,146 +2638,140 @@
         <v>146</v>
       </c>
     </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B97" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A98" t="s">
+      <c r="B98" s="1"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A99" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B99" s="1" t="s">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B100" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B100" s="1"/>
-    </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A101" t="s">
+      <c r="B101" s="1"/>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A102" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B102" s="1" t="s">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B103" s="1" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A105" t="s">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A106" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B106" s="1" t="s">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B107" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="K106" t="s">
+      <c r="K107" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="K107" t="s">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="K108" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A108" t="s">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A109" t="s">
         <v>159</v>
       </c>
-      <c r="K108" t="s">
+      <c r="K109" t="s">
         <v>162</v>
-      </c>
-    </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B109" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B110" s="1" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B111" s="1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B112" s="1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B112" s="1"/>
-    </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A113" t="s">
+      <c r="B113" s="1"/>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A114" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B114" s="1" t="s">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B115" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A116" t="s">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A117" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B117" s="1" t="s">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B118" s="1" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B118" s="1"/>
-    </row>
-    <row r="119" spans="1:11" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A119" s="5" t="s">
-        <v>156</v>
-      </c>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B119" s="1"/>
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
-        <v>137</v>
+        <v>360</v>
       </c>
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B121" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A122" s="5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A123" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B124" s="1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="20.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A124" s="5" t="s">
+    <row r="127" spans="1:11" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A127" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="K124" s="8" t="s">
+      <c r="K127" s="8" t="s">
         <v>211</v>
-      </c>
-    </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B125" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="K125" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B126" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="K126" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="B127" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="K127" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B128" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="K128" t="s">
         <v>209</v>
@@ -2678,30 +2779,54 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B129" s="1" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K129" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A130" t="s">
-        <v>168</v>
+      <c r="B130" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="K130" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B131" s="1" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
       <c r="K131" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.4">
       <c r="B132" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="K132" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A133" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B134" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="K134" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="B135" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="K132" t="s">
+      <c r="K135" t="s">
         <v>213</v>
       </c>
     </row>
@@ -2714,25 +2839,25 @@
     <hyperlink ref="B17" r:id="rId5" xr:uid="{7C53DCBF-69C4-47FA-A72D-2A48DBB11DF4}"/>
     <hyperlink ref="B40" r:id="rId6" xr:uid="{1BFC6B10-85CE-4E1B-B6B1-D8FA0CAABB34}"/>
     <hyperlink ref="B41" r:id="rId7" xr:uid="{9D30F7F2-B9FE-4D29-9495-F116DEF1F3A4}"/>
-    <hyperlink ref="B106" r:id="rId8" xr:uid="{7CFA9E65-A6DC-4DE8-AC9C-1AF423D38DFF}"/>
+    <hyperlink ref="B107" r:id="rId8" xr:uid="{7CFA9E65-A6DC-4DE8-AC9C-1AF423D38DFF}"/>
     <hyperlink ref="B77" r:id="rId9" xr:uid="{9B2EDC10-643B-4B9B-8FD5-96D0FFF647A0}"/>
-    <hyperlink ref="B121" r:id="rId10" xr:uid="{1616DA05-1E5D-4ABF-890C-20A07051790E}"/>
-    <hyperlink ref="B114" r:id="rId11" xr:uid="{BF99D095-4541-440D-AA7F-DA8EB65CC455}"/>
+    <hyperlink ref="B124" r:id="rId10" xr:uid="{1616DA05-1E5D-4ABF-890C-20A07051790E}"/>
+    <hyperlink ref="B115" r:id="rId11" xr:uid="{BF99D095-4541-440D-AA7F-DA8EB65CC455}"/>
     <hyperlink ref="B80" r:id="rId12" xr:uid="{1C3A32A4-438B-4632-A4FB-C69D687880F2}"/>
-    <hyperlink ref="B111" r:id="rId13" xr:uid="{FF11ECCF-2913-41D3-8828-401C0CE54292}"/>
-    <hyperlink ref="B102" r:id="rId14" location="url-route-registrations" xr:uid="{D35EA712-B463-4E77-AC0C-75C534CD4A91}"/>
+    <hyperlink ref="B112" r:id="rId13" xr:uid="{FF11ECCF-2913-41D3-8828-401C0CE54292}"/>
+    <hyperlink ref="B103" r:id="rId14" location="url-route-registrations" xr:uid="{D35EA712-B463-4E77-AC0C-75C534CD4A91}"/>
     <hyperlink ref="B91" r:id="rId15" xr:uid="{BE49B070-FEBB-43D1-A4EF-C84BDA031305}"/>
-    <hyperlink ref="B99" r:id="rId16" xr:uid="{B58923EB-7539-4084-81C9-E7977A612CE5}"/>
+    <hyperlink ref="B100" r:id="rId16" xr:uid="{B58923EB-7539-4084-81C9-E7977A612CE5}"/>
     <hyperlink ref="B57" r:id="rId17" xr:uid="{3368EF62-3F9A-4C12-9902-89AE351E1333}"/>
     <hyperlink ref="B63" r:id="rId18" xr:uid="{551D545E-000D-44CE-B388-5CDAD13376FD}"/>
     <hyperlink ref="B85" r:id="rId19" xr:uid="{458EBB60-0739-468E-AF59-58A8270D5827}"/>
     <hyperlink ref="B96" r:id="rId20" xr:uid="{95FC1958-A4CB-48ED-9019-782FF0B4A713}"/>
     <hyperlink ref="B39" r:id="rId21" xr:uid="{094F5B77-D00F-4A1F-BD30-F3AC196C7A30}"/>
-    <hyperlink ref="B109" r:id="rId22" xr:uid="{22858CD3-4B7F-4856-918F-9A27F355DFFB}"/>
-    <hyperlink ref="B110" r:id="rId23" location="url-route-registrations" xr:uid="{FE265927-EAA5-4CBE-B5F1-9FB6E72771B3}"/>
+    <hyperlink ref="B110" r:id="rId22" xr:uid="{22858CD3-4B7F-4856-918F-9A27F355DFFB}"/>
+    <hyperlink ref="B111" r:id="rId23" location="url-route-registrations" xr:uid="{FE265927-EAA5-4CBE-B5F1-9FB6E72771B3}"/>
     <hyperlink ref="B54" r:id="rId24" xr:uid="{7EA89C7F-C77C-4029-A969-1B84801049B8}"/>
-    <hyperlink ref="B132" r:id="rId25" xr:uid="{ECF08CCA-2051-458F-AAB1-F1430019D248}"/>
-    <hyperlink ref="B131" r:id="rId26" xr:uid="{33043EC6-6794-49B1-ACAA-9F669BB678EE}"/>
+    <hyperlink ref="B135" r:id="rId25" xr:uid="{ECF08CCA-2051-458F-AAB1-F1430019D248}"/>
+    <hyperlink ref="B134" r:id="rId26" xr:uid="{33043EC6-6794-49B1-ACAA-9F669BB678EE}"/>
     <hyperlink ref="B43" r:id="rId27" xr:uid="{8A59E9FD-A204-4740-9041-79338D62327F}"/>
     <hyperlink ref="B44" r:id="rId28" xr:uid="{B27E23E6-61AB-4065-BC6A-25A01A3CE5FC}"/>
     <hyperlink ref="B29" r:id="rId29" xr:uid="{3C068779-AD8A-4C4F-AC5D-D744816101F5}"/>
@@ -2740,11 +2865,11 @@
     <hyperlink ref="B21" r:id="rId31" xr:uid="{ABC21E56-52CD-4352-9A25-4F0A2391B569}"/>
     <hyperlink ref="B30" r:id="rId32" xr:uid="{D9B8F3BA-795D-4C78-BFC4-D863A3553642}"/>
     <hyperlink ref="B23" r:id="rId33" xr:uid="{93582230-84C1-43BE-BE89-41931B7ECA48}"/>
-    <hyperlink ref="B128" r:id="rId34" xr:uid="{9BFFB0C2-306D-4FE7-8010-112E866D0E32}"/>
-    <hyperlink ref="B129" r:id="rId35" xr:uid="{8A47A44B-B133-4903-92D9-092FA9C1578D}"/>
-    <hyperlink ref="B126" r:id="rId36" xr:uid="{EF6F40D0-2771-4CAF-9E58-70583011CCE9}"/>
-    <hyperlink ref="B125" r:id="rId37" xr:uid="{E6BCEFF2-BAB8-4CB8-80EF-D7C55D3E95F3}"/>
-    <hyperlink ref="B127" r:id="rId38" xr:uid="{6F3DB4D3-50D4-4D30-9DE3-A407A1575FA3}"/>
+    <hyperlink ref="B131" r:id="rId34" xr:uid="{9BFFB0C2-306D-4FE7-8010-112E866D0E32}"/>
+    <hyperlink ref="B132" r:id="rId35" xr:uid="{8A47A44B-B133-4903-92D9-092FA9C1578D}"/>
+    <hyperlink ref="B129" r:id="rId36" xr:uid="{EF6F40D0-2771-4CAF-9E58-70583011CCE9}"/>
+    <hyperlink ref="B128" r:id="rId37" xr:uid="{E6BCEFF2-BAB8-4CB8-80EF-D7C55D3E95F3}"/>
+    <hyperlink ref="B130" r:id="rId38" xr:uid="{6F3DB4D3-50D4-4D30-9DE3-A407A1575FA3}"/>
     <hyperlink ref="B61" r:id="rId39" xr:uid="{B667A22F-F780-4881-B207-E72497E5B988}"/>
     <hyperlink ref="B67" r:id="rId40" xr:uid="{E6028D46-536F-4F56-9548-4856CEB07885}"/>
     <hyperlink ref="B65" r:id="rId41" xr:uid="{6A3C338D-3F85-48DC-BA24-34726D4947B8}"/>
@@ -2757,21 +2882,23 @@
     <hyperlink ref="B36" r:id="rId48" location="advanced" xr:uid="{BA770625-6172-4CFA-99A6-033BBE6A8889}"/>
     <hyperlink ref="B47" r:id="rId49" xr:uid="{1E8CEAB3-1AC4-4E7E-A34A-4EA09801E259}"/>
     <hyperlink ref="B50" r:id="rId50" xr:uid="{3DB406F9-ECB0-465E-85D9-CF98A5834D8E}"/>
-    <hyperlink ref="B117" r:id="rId51" xr:uid="{CDE876B4-A028-43CE-B1CE-8313986B8A5F}"/>
+    <hyperlink ref="B118" r:id="rId51" xr:uid="{CDE876B4-A028-43CE-B1CE-8313986B8A5F}"/>
     <hyperlink ref="B88" r:id="rId52" xr:uid="{8AE1F483-3F49-49DC-8BD3-4C0DA20FE198}"/>
     <hyperlink ref="K91" r:id="rId53" xr:uid="{523F07D4-16FB-452A-B926-E319A680D6CA}"/>
+    <hyperlink ref="B121" r:id="rId54" xr:uid="{36D70757-F7F2-4E5A-A543-AE39B6684213}"/>
+    <hyperlink ref="B97" r:id="rId55" xr:uid="{4FC0045E-3022-473C-ACA6-39112DB6A257}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE686A04-9AA8-4B6B-ADC4-7F706D929E57}">
-  <dimension ref="A3:H165"/>
+  <dimension ref="A3:J165"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3100,17 +3227,17 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B65" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.4">
       <c r="E66" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B67" t="s">
         <v>14</v>
       </c>
@@ -3133,7 +3260,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.4">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B68" t="s">
         <v>3</v>
       </c>
@@ -3156,8 +3283,11 @@
       <c r="H68" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J68" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B69" t="s">
         <v>4</v>
       </c>
@@ -3168,8 +3298,11 @@
         <f>B69 &amp; "@" &amp; $B$60</f>
         <v>employee02@tony-held.com</v>
       </c>
-    </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J69" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B70" t="s">
         <v>5</v>
       </c>
@@ -3180,8 +3313,11 @@
         <f>B70 &amp; "@" &amp; $B$60</f>
         <v>employee03@tony-held.com</v>
       </c>
-    </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J70" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B71" t="s">
         <v>6</v>
       </c>
@@ -3192,8 +3328,11 @@
         <f>B71 &amp; "@" &amp; $B$60</f>
         <v>employee04@tony-held.com</v>
       </c>
-    </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J71" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B72" t="s">
         <v>7</v>
       </c>
@@ -3204,8 +3343,11 @@
         <f>B72 &amp; "@" &amp; $B$60</f>
         <v>employee05@tony-held.com</v>
       </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J72" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B74" t="s">
         <v>8</v>
       </c>
@@ -3216,8 +3358,11 @@
         <f>B74 &amp; "@" &amp; $B$60</f>
         <v>patient01@tony-held.com</v>
       </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J74" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B75" t="s">
         <v>9</v>
       </c>
@@ -3228,8 +3373,11 @@
         <f>B75 &amp; "@" &amp; $B$60</f>
         <v>patient02@tony-held.com</v>
       </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J75" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B76" t="s">
         <v>10</v>
       </c>
@@ -3240,8 +3388,11 @@
         <f>B76 &amp; "@" &amp; $B$60</f>
         <v>patient03@tony-held.com</v>
       </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J76" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B77" t="s">
         <v>11</v>
       </c>
@@ -3252,8 +3403,11 @@
         <f>B77 &amp; "@" &amp; $B$60</f>
         <v>patient04@tony-held.com</v>
       </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.4">
+      <c r="J77" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.4">
       <c r="B78" t="s">
         <v>12</v>
       </c>
@@ -3263,6 +3417,9 @@
       <c r="D78" t="str">
         <f>B78 &amp; "@" &amp; $B$60</f>
         <v>patient05@tony-held.com</v>
+      </c>
+      <c r="J78" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.4">
@@ -3765,9 +3922,10 @@
     <hyperlink ref="B134" r:id="rId21" xr:uid="{2AA9B621-7D9C-4C88-894A-5115FE5D074C}"/>
     <hyperlink ref="B139" r:id="rId22" xr:uid="{A349F0C4-93D2-428A-AFD6-797BE646EC6B}"/>
     <hyperlink ref="B161" r:id="rId23" location="a-minimal-application" xr:uid="{02EDAFF4-690A-44FD-AE5B-5AEFF014D3E2}"/>
+    <hyperlink ref="J68" r:id="rId24" xr:uid="{1098846A-1C7D-42BC-A292-F7174F05C075}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId24"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>

</xml_diff>